<commit_message>
optimised retail fee calcs
</commit_message>
<xml_diff>
--- a/INPUT DATA/Tariff Type.xlsx
+++ b/INPUT DATA/Tariff Type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josea\Documents\HooRah\RMIT\Capstone\Python\Pricing Model\GRAPHY_SIMPLE\INPUT DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00700C65-54BC-4AB1-ABEE-BCE93478E1AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4DD0AE-4956-4384-AB50-C08B021EF667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tariff2" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,30 @@
     <sheet name="Tariff13" sheetId="3" r:id="rId3"/>
     <sheet name="Tariff14" sheetId="4" r:id="rId4"/>
     <sheet name="TariffNDM" sheetId="5" r:id="rId5"/>
+    <sheet name="TariffLLV" sheetId="6" r:id="rId6"/>
+    <sheet name="TariffND5" sheetId="7" r:id="rId7"/>
+    <sheet name="FacilityIndex" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>Time</t>
   </si>
@@ -54,13 +66,121 @@
   <si>
     <t>Saturday</t>
   </si>
+  <si>
+    <t>Wodonga Head Office</t>
+  </si>
+  <si>
+    <t>Wodonga Water Treatment Plant</t>
+  </si>
+  <si>
+    <t>Yarrawonga Wastewater Winter Storage - Irrigation</t>
+  </si>
+  <si>
+    <t>Wahgunyah Water Treatment Plant</t>
+  </si>
+  <si>
+    <t>Yarrawonga Water Treatment Plant</t>
+  </si>
+  <si>
+    <t>Benalla Water Treatment Plant</t>
+  </si>
+  <si>
+    <t>Myrtleford Wastewater Purification Plant - Area 2 (Depot)</t>
+  </si>
+  <si>
+    <t>Myrtleford Water Treatment Plant &amp; Reservoir</t>
+  </si>
+  <si>
+    <t>Wodonga (Baranduda) Wastewater Purification Plant</t>
+  </si>
+  <si>
+    <t>Wangaratta Offtake / Treatment Plant / Distribution Pumping</t>
+  </si>
+  <si>
+    <t>Benalla Wastewater Purification Plant / Farm</t>
+  </si>
+  <si>
+    <t>Bright Wastewater Purification Plant</t>
+  </si>
+  <si>
+    <t>Wangaratta Wastewater Purification Plant</t>
+  </si>
+  <si>
+    <t>Wangaratta Kerr St Tanks</t>
+  </si>
+  <si>
+    <t>Wahgunyah Wastewater Purification Plant</t>
+  </si>
+  <si>
+    <t>Wodonga West Wod Wastewater Purification Plant</t>
+  </si>
+  <si>
+    <t>Corryong Water Treatment Plant - Water Storage 3</t>
+  </si>
+  <si>
+    <t>Wangaratta Trade Waste Treatment Plant</t>
+  </si>
+  <si>
+    <t>Mount Beauty Wastewater Purification Plant</t>
+  </si>
+  <si>
+    <t>Bright Water Treatment Plant &amp; Off stream storage</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Baranduda Low Level Water Pump Station</t>
+  </si>
+  <si>
+    <t>Wangaratta - Phillipson St Storage  Clear Water Pump Station</t>
+  </si>
+  <si>
+    <t>Wodonga Raw Water Pump Station</t>
+  </si>
+  <si>
+    <t>Wodonga Pump Station 01</t>
+  </si>
+  <si>
+    <t>Bright Hawthorn Lane Sewer pump station</t>
+  </si>
+  <si>
+    <t>Myrtleford Buffalo Creek Sewer Pump Station</t>
+  </si>
+  <si>
+    <t>Wangaratta Swan St Sewer Pump Station</t>
+  </si>
+  <si>
+    <t>Corryong Offtake Sewer Pump Station (Nariel Creek)</t>
+  </si>
+  <si>
+    <t>Wodonga High Level Water Pump Station</t>
+  </si>
+  <si>
+    <t>Yarrawonga Offtake Pump station</t>
+  </si>
+  <si>
+    <t>Non Potable Offtake Water Pump Station (purple pipe)</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -93,23 +213,12 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1723,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1167A657-1973-47EF-847E-ECEF5D93EA32}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3060,7 +3169,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3721,4 +3830,1916 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B7B25C-A8A0-4704-8D36-F84C2FCF4670}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC7FD26-76CA-474D-A9F1-F35B71971D2B}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F7EA1D-230F-4B6A-8E1D-4A3B217FBA0E}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>26</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <v>18</v>
+      </c>
+      <c r="E24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>